<commit_message>
Model - need fix lasso
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>Ann mean</t>
   </si>
@@ -30,6 +30,9 @@
   </si>
   <si>
     <t>Ann Sharpe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food </t>
   </si>
   <si>
     <t xml:space="preserve">Beer </t>
@@ -465,7 +468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,19 +498,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>7.200524858147883</v>
+        <v>8.28858394160584</v>
       </c>
       <c r="C2" t="n">
-        <v>17.62014570764966</v>
+        <v>15.02256728639485</v>
       </c>
       <c r="D2" t="n">
-        <v>-20.19</v>
+        <v>-18.15</v>
       </c>
       <c r="E2" t="n">
-        <v>25.51</v>
+        <v>19.89</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4086529690286175</v>
+        <v>0.5517421745291416</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -515,19 +518,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>10.01465930039973</v>
+        <v>8.527357664233577</v>
       </c>
       <c r="C3" t="n">
-        <v>20.98260418565459</v>
+        <v>17.62014570764966</v>
       </c>
       <c r="D3" t="n">
-        <v>-25.32</v>
+        <v>-20.19</v>
       </c>
       <c r="E3" t="n">
-        <v>32.38</v>
+        <v>25.51</v>
       </c>
       <c r="F3" t="n">
-        <v>0.4772839067920162</v>
+        <v>0.4839550027404988</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -535,19 +538,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>5.40308906178586</v>
+        <v>11.78785401459854</v>
       </c>
       <c r="C4" t="n">
-        <v>24.85726650559794</v>
+        <v>20.98260418565459</v>
       </c>
       <c r="D4" t="n">
-        <v>-33.4</v>
+        <v>-25.32</v>
       </c>
       <c r="E4" t="n">
-        <v>34.52</v>
+        <v>32.38</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2173645706606181</v>
+        <v>0.5617917542693615</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -555,19 +558,19 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>4.395269112902556</v>
+        <v>8.420496350364957</v>
       </c>
       <c r="C5" t="n">
-        <v>20.10935974137821</v>
+        <v>24.85726650559794</v>
       </c>
       <c r="D5" t="n">
-        <v>-26.56</v>
+        <v>-33.4</v>
       </c>
       <c r="E5" t="n">
-        <v>33.13</v>
+        <v>34.52</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2185683268601828</v>
+        <v>0.3387539152170506</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -575,19 +578,19 @@
         <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>5.409849975912917</v>
+        <v>6.339328467153287</v>
       </c>
       <c r="C6" t="n">
-        <v>16.47664660552681</v>
+        <v>20.10935974137821</v>
       </c>
       <c r="D6" t="n">
-        <v>-22.24</v>
+        <v>-26.56</v>
       </c>
       <c r="E6" t="n">
-        <v>18.22</v>
+        <v>33.13</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3283344059887935</v>
+        <v>0.3152426804573548</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -595,19 +598,19 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>5.717003510652763</v>
+        <v>6.650277372262765</v>
       </c>
       <c r="C7" t="n">
-        <v>22.10569470513691</v>
+        <v>16.47664660552681</v>
       </c>
       <c r="D7" t="n">
-        <v>-31.5</v>
+        <v>-22.24</v>
       </c>
       <c r="E7" t="n">
-        <v>31.79</v>
+        <v>18.22</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2586213003893629</v>
+        <v>0.4036183776638168</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -615,19 +618,19 @@
         <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>6.546287188493261</v>
+        <v>8.033518248175184</v>
       </c>
       <c r="C8" t="n">
-        <v>17.05887801763106</v>
+        <v>22.10569470513691</v>
       </c>
       <c r="D8" t="n">
-        <v>-21.06</v>
+        <v>-31.5</v>
       </c>
       <c r="E8" t="n">
-        <v>29.01</v>
+        <v>31.79</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3837466439309432</v>
+        <v>0.3634139689040561</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -635,19 +638,19 @@
         <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>4.491725060140905</v>
+        <v>7.810861313868612</v>
       </c>
       <c r="C9" t="n">
-        <v>19.10260565426213</v>
+        <v>17.05887801763106</v>
       </c>
       <c r="D9" t="n">
-        <v>-28.6</v>
+        <v>-21.06</v>
       </c>
       <c r="E9" t="n">
-        <v>21.68</v>
+        <v>29.01</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2351367735604552</v>
+        <v>0.4578766144992515</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -655,19 +658,19 @@
         <v>13</v>
       </c>
       <c r="B10" t="n">
-        <v>5.188819867176986</v>
+        <v>6.23737226277372</v>
       </c>
       <c r="C10" t="n">
-        <v>24.30906902099031</v>
+        <v>19.10260565426213</v>
       </c>
       <c r="D10" t="n">
-        <v>-33.11</v>
+        <v>-28.6</v>
       </c>
       <c r="E10" t="n">
-        <v>59.03</v>
+        <v>21.68</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2134520191907211</v>
+        <v>0.3265194484806868</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -675,19 +678,19 @@
         <v>14</v>
       </c>
       <c r="B11" t="n">
-        <v>4.183561309003503</v>
+        <v>8.00899270072992</v>
       </c>
       <c r="C11" t="n">
-        <v>20.73950268645295</v>
+        <v>24.30906902099031</v>
       </c>
       <c r="D11" t="n">
-        <v>-28.74</v>
+        <v>-33.11</v>
       </c>
       <c r="E11" t="n">
-        <v>25.02</v>
+        <v>59.03</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2017194612740741</v>
+        <v>0.3294652170272067</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -695,19 +698,19 @@
         <v>15</v>
       </c>
       <c r="B12" t="n">
-        <v>0.297347405259818</v>
+        <v>6.281518248175189</v>
       </c>
       <c r="C12" t="n">
-        <v>25.2542486174469</v>
+        <v>20.73950268645295</v>
       </c>
       <c r="D12" t="n">
-        <v>-32.98999999999999</v>
+        <v>-28.74</v>
       </c>
       <c r="E12" t="n">
-        <v>30.36</v>
+        <v>25.02</v>
       </c>
       <c r="F12" t="n">
-        <v>0.01177415371821419</v>
+        <v>0.3028769948412639</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -715,19 +718,19 @@
         <v>16</v>
       </c>
       <c r="B13" t="n">
-        <v>4.561461250662835</v>
+        <v>3.543591240875913</v>
       </c>
       <c r="C13" t="n">
-        <v>21.16453811108553</v>
+        <v>25.2542486174469</v>
       </c>
       <c r="D13" t="n">
-        <v>-31.63</v>
+        <v>-32.98999999999999</v>
       </c>
       <c r="E13" t="n">
-        <v>22.91</v>
+        <v>30.36</v>
       </c>
       <c r="F13" t="n">
-        <v>0.2155237797641159</v>
+        <v>0.1403166371945758</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -735,19 +738,19 @@
         <v>17</v>
       </c>
       <c r="B14" t="n">
-        <v>6.292683968342527</v>
+        <v>6.75100729927007</v>
       </c>
       <c r="C14" t="n">
-        <v>21.50160936722616</v>
+        <v>21.16453811108553</v>
       </c>
       <c r="D14" t="n">
-        <v>-32.8</v>
+        <v>-31.63</v>
       </c>
       <c r="E14" t="n">
-        <v>23.21</v>
+        <v>22.91</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2926610683353849</v>
+        <v>0.3189773036310222</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -755,19 +758,19 @@
         <v>18</v>
       </c>
       <c r="B15" t="n">
-        <v>2.796311131870466</v>
+        <v>8.450627737226274</v>
       </c>
       <c r="C15" t="n">
-        <v>23.15473826233936</v>
+        <v>21.50160936722616</v>
       </c>
       <c r="D15" t="n">
-        <v>-36.48999999999999</v>
+        <v>-32.8</v>
       </c>
       <c r="E15" t="n">
-        <v>49.56</v>
+        <v>23.21</v>
       </c>
       <c r="F15" t="n">
-        <v>0.120766259596145</v>
+        <v>0.3930230334342855</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -775,19 +778,19 @@
         <v>19</v>
       </c>
       <c r="B16" t="n">
-        <v>6.399062365777919</v>
+        <v>5.447824817518251</v>
       </c>
       <c r="C16" t="n">
-        <v>21.78318558474901</v>
+        <v>23.15473826233936</v>
       </c>
       <c r="D16" t="n">
-        <v>-31.1</v>
+        <v>-36.48999999999999</v>
       </c>
       <c r="E16" t="n">
-        <v>23.39</v>
+        <v>49.56</v>
       </c>
       <c r="F16" t="n">
-        <v>0.2937615502049467</v>
+        <v>0.2352790498340036</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -795,19 +798,19 @@
         <v>20</v>
       </c>
       <c r="B17" t="n">
-        <v>3.252748748619472</v>
+        <v>8.624759124087598</v>
       </c>
       <c r="C17" t="n">
-        <v>25.79868927730801</v>
+        <v>21.78318558474901</v>
       </c>
       <c r="D17" t="n">
-        <v>-34.55</v>
+        <v>-31.1</v>
       </c>
       <c r="E17" t="n">
-        <v>35.15</v>
+        <v>23.39</v>
       </c>
       <c r="F17" t="n">
-        <v>0.1260819382587984</v>
+        <v>0.3959365397008792</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -815,19 +818,19 @@
         <v>21</v>
       </c>
       <c r="B18" t="n">
-        <v>2.607522693047581</v>
+        <v>6.583883211678836</v>
       </c>
       <c r="C18" t="n">
-        <v>35.28518769141299</v>
+        <v>25.79868927730801</v>
       </c>
       <c r="D18" t="n">
-        <v>-38.09</v>
+        <v>-34.55</v>
       </c>
       <c r="E18" t="n">
-        <v>45.55</v>
+        <v>35.15</v>
       </c>
       <c r="F18" t="n">
-        <v>0.07389850709741722</v>
+        <v>0.2552022368620829</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -835,19 +838,19 @@
         <v>22</v>
       </c>
       <c r="B19" t="n">
-        <v>6.274778434850758</v>
+        <v>8.826569343065701</v>
       </c>
       <c r="C19" t="n">
-        <v>18.51382999080828</v>
+        <v>35.28518769141299</v>
       </c>
       <c r="D19" t="n">
-        <v>-18.96</v>
+        <v>-38.09</v>
       </c>
       <c r="E19" t="n">
-        <v>23.7</v>
+        <v>45.55</v>
       </c>
       <c r="F19" t="n">
-        <v>0.3389238443890892</v>
+        <v>0.250149423045686</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -855,19 +858,19 @@
         <v>23</v>
       </c>
       <c r="B20" t="n">
-        <v>4.951279809549258</v>
+        <v>7.811737226277371</v>
       </c>
       <c r="C20" t="n">
-        <v>13.81046884056616</v>
+        <v>18.51382999080828</v>
       </c>
       <c r="D20" t="n">
-        <v>-12.94</v>
+        <v>-18.96</v>
       </c>
       <c r="E20" t="n">
-        <v>18.26</v>
+        <v>23.7</v>
       </c>
       <c r="F20" t="n">
-        <v>0.3585164172707608</v>
+        <v>0.421940637358976</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -875,19 +878,19 @@
         <v>24</v>
       </c>
       <c r="B21" t="n">
-        <v>5.086787787182923</v>
+        <v>5.797489051094894</v>
       </c>
       <c r="C21" t="n">
-        <v>16.02405172125827</v>
+        <v>13.81046884056616</v>
       </c>
       <c r="D21" t="n">
-        <v>-16.44</v>
+        <v>-12.94</v>
       </c>
       <c r="E21" t="n">
-        <v>21.22</v>
+        <v>18.26</v>
       </c>
       <c r="F21" t="n">
-        <v>0.3174470399664616</v>
+        <v>0.4197894450958571</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -895,19 +898,19 @@
         <v>25</v>
       </c>
       <c r="B22" t="n">
-        <v>5.777618351293845</v>
+        <v>6.260846715328465</v>
       </c>
       <c r="C22" t="n">
-        <v>22.5910189013917</v>
+        <v>16.02405172125827</v>
       </c>
       <c r="D22" t="n">
-        <v>-28.67</v>
+        <v>-16.44</v>
       </c>
       <c r="E22" t="n">
-        <v>23.38</v>
+        <v>21.22</v>
       </c>
       <c r="F22" t="n">
-        <v>0.2557484625422504</v>
+        <v>0.390715583314208</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -915,19 +918,19 @@
         <v>26</v>
       </c>
       <c r="B23" t="n">
-        <v>4.277403434071037</v>
+        <v>8.200992700729923</v>
       </c>
       <c r="C23" t="n">
-        <v>23.32489272997021</v>
+        <v>22.5910189013917</v>
       </c>
       <c r="D23" t="n">
-        <v>-32.07</v>
+        <v>-28.67</v>
       </c>
       <c r="E23" t="n">
-        <v>24.66</v>
+        <v>23.38</v>
       </c>
       <c r="F23" t="n">
-        <v>0.1833836272513696</v>
+        <v>0.3630200451129147</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -935,19 +938,19 @@
         <v>27</v>
       </c>
       <c r="B24" t="n">
-        <v>4.677587516724535</v>
+        <v>6.965781021897816</v>
       </c>
       <c r="C24" t="n">
-        <v>17.49821938737792</v>
+        <v>23.32489272997021</v>
       </c>
       <c r="D24" t="n">
-        <v>-27.74</v>
+        <v>-32.07</v>
       </c>
       <c r="E24" t="n">
-        <v>21</v>
+        <v>24.66</v>
       </c>
       <c r="F24" t="n">
-        <v>0.2673179146501412</v>
+        <v>0.2986415029873843</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -955,19 +958,19 @@
         <v>28</v>
       </c>
       <c r="B25" t="n">
-        <v>5.136531586608073</v>
+        <v>6.120525547445252</v>
       </c>
       <c r="C25" t="n">
-        <v>19.84233892676217</v>
+        <v>17.49821938737792</v>
       </c>
       <c r="D25" t="n">
-        <v>-28.32</v>
+        <v>-27.74</v>
       </c>
       <c r="E25" t="n">
-        <v>19.08</v>
+        <v>21</v>
       </c>
       <c r="F25" t="n">
-        <v>0.2588672437038269</v>
+        <v>0.3497799068549914</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -975,19 +978,19 @@
         <v>29</v>
       </c>
       <c r="B26" t="n">
-        <v>5.705583536864056</v>
+        <v>7.006598540145987</v>
       </c>
       <c r="C26" t="n">
-        <v>19.4030821681548</v>
+        <v>19.84233892676217</v>
       </c>
       <c r="D26" t="n">
-        <v>-29.25</v>
+        <v>-28.32</v>
       </c>
       <c r="E26" t="n">
-        <v>17.53</v>
+        <v>19.08</v>
       </c>
       <c r="F26" t="n">
-        <v>0.2940555262002813</v>
+        <v>0.3531135399917951</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -995,19 +998,19 @@
         <v>30</v>
       </c>
       <c r="B27" t="n">
-        <v>6.425804825627912</v>
+        <v>7.471883211678826</v>
       </c>
       <c r="C27" t="n">
-        <v>18.51853980211666</v>
+        <v>19.4030821681548</v>
       </c>
       <c r="D27" t="n">
-        <v>-29.74</v>
+        <v>-29.25</v>
       </c>
       <c r="E27" t="n">
-        <v>26.49</v>
+        <v>17.53</v>
       </c>
       <c r="F27" t="n">
-        <v>0.3469930617798194</v>
+        <v>0.3850874385277825</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1015,19 +1018,19 @@
         <v>31</v>
       </c>
       <c r="B28" t="n">
-        <v>6.363041034178973</v>
+        <v>7.972554744525541</v>
       </c>
       <c r="C28" t="n">
-        <v>21.13288775493542</v>
+        <v>18.51853980211666</v>
       </c>
       <c r="D28" t="n">
-        <v>-31.89</v>
+        <v>-29.74</v>
       </c>
       <c r="E28" t="n">
-        <v>27.38</v>
+        <v>26.49</v>
       </c>
       <c r="F28" t="n">
-        <v>0.3010966181227616</v>
+        <v>0.4305174614045045</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1035,19 +1038,19 @@
         <v>32</v>
       </c>
       <c r="B29" t="n">
-        <v>5.674967727719915</v>
+        <v>8.467795620437951</v>
       </c>
       <c r="C29" t="n">
-        <v>18.73319584034935</v>
+        <v>21.13288775493542</v>
       </c>
       <c r="D29" t="n">
-        <v>-22.53</v>
+        <v>-31.89</v>
       </c>
       <c r="E29" t="n">
-        <v>20.59</v>
+        <v>27.38</v>
       </c>
       <c r="F29" t="n">
-        <v>0.3029364437378393</v>
+        <v>0.4006927836192365</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1055,19 +1058,39 @@
         <v>33</v>
       </c>
       <c r="B30" t="n">
-        <v>2.489632682606024</v>
+        <v>7.310715328467154</v>
       </c>
       <c r="C30" t="n">
+        <v>18.73319584034935</v>
+      </c>
+      <c r="D30" t="n">
+        <v>-22.53</v>
+      </c>
+      <c r="E30" t="n">
+        <v>20.59</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.3902545721921423</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="n">
+        <v>4.529167883211674</v>
+      </c>
+      <c r="C31" t="n">
         <v>20.15123387703878</v>
       </c>
-      <c r="D30" t="n">
+      <c r="D31" t="n">
         <v>-28.09</v>
       </c>
-      <c r="E30" t="n">
+      <c r="E31" t="n">
         <v>19.96</v>
       </c>
-      <c r="F30" t="n">
-        <v>0.1235474064664012</v>
+      <c r="F31" t="n">
+        <v>0.2247588366473386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>